<commit_message>
Fixed invalid entry in requirements.txt
</commit_message>
<xml_diff>
--- a/Book1.xlsx
+++ b/Book1.xlsx
@@ -595,7 +595,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M14"/>
+  <dimension ref="A1:M16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="M11" sqref="M11"/>
@@ -1263,6 +1263,100 @@
         </is>
       </c>
     </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>4CH3Z</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>11/29/2024</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>Ashar Nadeem</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>0322-7287568</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>Lahore</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>0322-7287568</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>xxdxsdxdsx</t>
+        </is>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>csssdccs</t>
+        </is>
+      </c>
+      <c r="I15" t="inlineStr">
+        <is>
+          <t>cscsd</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>BXMIY</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>11/29/2024</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>Medum masala chai</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>0322-7287568</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>Lahore</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>0322-7287568</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>cscdcd</t>
+        </is>
+      </c>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>csssdccs</t>
+        </is>
+      </c>
+      <c r="I16" t="inlineStr">
+        <is>
+          <t>cdcdscd</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="5">
     <mergeCell ref="L3:M3"/>

</xml_diff>